<commit_message>
Added single qubit classifier and analysis
</commit_message>
<xml_diff>
--- a/exp2/exp2A_results.xlsx
+++ b/exp2/exp2A_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31642\Documents\GRONINGEN\PROJECT\Code\exp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CF0A85-B55A-4187-BB82-EA1626E32A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C63C708-6C6F-4B05-B693-485C34208346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31845" yWindow="1005" windowWidth="13635" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Als de max en mean een andere beste LR hebben is het verschil tussen de means voor de twee lrs meestal klein (.01)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>With crossvalidation</t>
   </si>
 </sst>
 </file>
@@ -381,155 +387,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I8"/>
+  <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
+        <v>0.46</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
         <v>0.72</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>0.1</v>
       </c>
-      <c r="E3">
-        <v>0.46</v>
-      </c>
-      <c r="F3">
-        <v>0.05</v>
-      </c>
-      <c r="G3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.05</v>
+      </c>
+      <c r="E4">
+        <v>0.44</v>
+      </c>
+      <c r="F4">
         <v>0.9</v>
       </c>
-      <c r="D4">
-        <v>0.05</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
-      </c>
-      <c r="F4">
-        <v>0.05</v>
-      </c>
       <c r="G4">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.84</v>
+        <v>0.52</v>
       </c>
       <c r="D5">
         <v>0.01</v>
       </c>
       <c r="E5">
-        <v>0.52</v>
+        <v>0.12</v>
       </c>
       <c r="F5">
+        <v>0.84</v>
+      </c>
+      <c r="G5">
         <v>0.01</v>
-      </c>
-      <c r="G5">
-        <v>0.12</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
+        <v>0.45</v>
+      </c>
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <v>0.21</v>
+      </c>
+      <c r="F6">
         <v>0.78</v>
       </c>
-      <c r="D6">
-        <v>0.05</v>
-      </c>
-      <c r="E6">
-        <v>0.45</v>
-      </c>
-      <c r="F6">
-        <v>0.05</v>
-      </c>
       <c r="G6">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
+        <v>0.44</v>
+      </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
+      <c r="E7">
+        <v>0.21</v>
+      </c>
+      <c r="F7">
         <v>0.89</v>
       </c>
-      <c r="D7">
-        <v>0.05</v>
-      </c>
-      <c r="E7">
-        <v>0.44</v>
-      </c>
-      <c r="F7">
-        <v>0.01</v>
-      </c>
       <c r="G7">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
-        <v>0.92</v>
+        <v>0.43</v>
       </c>
       <c r="D8">
         <v>0.01</v>
       </c>
       <c r="E8">
-        <v>0.43</v>
+        <v>0.22</v>
       </c>
       <c r="F8">
+        <v>0.92</v>
+      </c>
+      <c r="G8">
         <v>0.01</v>
       </c>
-      <c r="G8">
-        <v>0.22</v>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0.72</v>
+      </c>
+      <c r="D12">
+        <v>0.05</v>
+      </c>
+      <c r="E12">
+        <v>0.45</v>
+      </c>
+      <c r="F12">
+        <v>0.95</v>
+      </c>
+      <c r="G12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0.89</v>
+      </c>
+      <c r="D13">
+        <v>0.05</v>
+      </c>
+      <c r="E13">
+        <v>0.06</v>
+      </c>
+      <c r="F13">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0.88</v>
+      </c>
+      <c r="E14">
+        <v>0.06</v>
+      </c>
+      <c r="F14">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0.53</v>
+      </c>
+      <c r="E15">
+        <v>0.08</v>
+      </c>
+      <c r="F15">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>0.88</v>
+      </c>
+      <c r="E16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0.9</v>
+      </c>
+      <c r="E17">
+        <v>0.06</v>
+      </c>
+      <c r="F17">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>